<commit_message>
updates as of draft version 3.2
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/stefanie_lane_ubc_ca/Documents/Documents/Dissertation/CommunityStability/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slane84\OneDrive - The University Of British Columbia\Documents\Dissertation\CommunityStability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{D7D29953-1664-4D93-B392-574D2E7B9CD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="14_{D7D29953-1664-4D93-B392-574D2E7B9CD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0CE04E9A-9FD3-4A7A-9B7B-F065C4BEFC58}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{D5046F42-BD19-457B-A65F-4703A2C409A5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="316">
   <si>
     <t>IndVal</t>
   </si>
@@ -850,45 +850,24 @@
     <t>Sidalcia_hendersonii</t>
   </si>
   <si>
-    <t>spelling - Puccinellia</t>
-  </si>
-  <si>
-    <t>Puccinella_pauciflora</t>
-  </si>
-  <si>
-    <t>Trifolium_wormskioldii</t>
-  </si>
-  <si>
     <t>Potentilla_pacifica</t>
   </si>
   <si>
-    <t>Symphotrichum_subspicatum</t>
-  </si>
-  <si>
     <t>Polygonum_hydropiper</t>
   </si>
   <si>
     <t>Poa_trivialis</t>
   </si>
   <si>
-    <t>Schoenoplectus_tabernaemontani</t>
-  </si>
-  <si>
     <t>Poa_palustris</t>
   </si>
   <si>
-    <t>Scirpus_microcarpus</t>
-  </si>
-  <si>
     <t>Platanthera_dilatata</t>
   </si>
   <si>
     <t>Poa_cf_palustris</t>
   </si>
   <si>
-    <t>Salix_scouleriana</t>
-  </si>
-  <si>
     <t>Phalaris_arundinacea</t>
   </si>
   <si>
@@ -913,9 +892,6 @@
     <t>Mentha_citrata</t>
   </si>
   <si>
-    <t>Platanthera_dilatata_var_dilatata</t>
-  </si>
-  <si>
     <t>Mentha_arvensis</t>
   </si>
   <si>
@@ -925,9 +901,6 @@
     <t>Lysimachia_thyrsiflora</t>
   </si>
   <si>
-    <t>Myrica_gale</t>
-  </si>
-  <si>
     <t>Lilaeopsis_occidentalis</t>
   </si>
   <si>
@@ -943,9 +916,6 @@
     <t>Leersia_oryzoides</t>
   </si>
   <si>
-    <t>Mentha_aquatica</t>
-  </si>
-  <si>
     <t>Lathyrus_palustris</t>
   </si>
   <si>
@@ -958,15 +928,9 @@
     <t>Juncus_articulatus</t>
   </si>
   <si>
-    <t>Lycopus_europaeus</t>
-  </si>
-  <si>
     <t>Iris_pseudocorus</t>
   </si>
   <si>
-    <t>Lysichiton_americanus</t>
-  </si>
-  <si>
     <t>Impatiens_capensis</t>
   </si>
   <si>
@@ -991,42 +955,27 @@
     <t>Galium_sp</t>
   </si>
   <si>
-    <t>code should be JUAR4</t>
-  </si>
-  <si>
     <t>Festuca_sp</t>
   </si>
   <si>
     <t>Festuca_arundinacea</t>
   </si>
   <si>
-    <t>Juncus_acuminatus</t>
-  </si>
-  <si>
     <t>Equisetum_variegatum</t>
   </si>
   <si>
-    <t>Iris_pseudacorus</t>
-  </si>
-  <si>
     <t>Equisetum_palustre</t>
   </si>
   <si>
     <t>Equisetum_fluviatile</t>
   </si>
   <si>
-    <t>Hypericum_scouleri</t>
-  </si>
-  <si>
     <t>Eleocharis_palustris</t>
   </si>
   <si>
     <t>Deschampsia_caespitosa</t>
   </si>
   <si>
-    <t>Galium_trifidum</t>
-  </si>
-  <si>
     <t>GATR2</t>
   </si>
   <si>
@@ -1036,21 +985,12 @@
     <t>Composite_unidentif</t>
   </si>
   <si>
-    <t>Galium_palustre</t>
-  </si>
-  <si>
     <t>Cirsium_arvense</t>
   </si>
   <si>
-    <t>syn Schedonorus arundinaceus</t>
-  </si>
-  <si>
     <t>Carex_lyngbei</t>
   </si>
   <si>
-    <t>Equisetum_arvense</t>
-  </si>
-  <si>
     <t>Caltha_palustris</t>
   </si>
   <si>
@@ -1078,16 +1018,172 @@
     <t>Agrostis_alba</t>
   </si>
   <si>
-    <t>Agrostis_stolonifera</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
-    <t>code</t>
-  </si>
-  <si>
     <t>Sidalcea hendersonii</t>
+  </si>
+  <si>
+    <t>JUAR4</t>
+  </si>
+  <si>
+    <t>NRCS Plant Code</t>
+  </si>
+  <si>
+    <t>Puccinellia_pauciflora</t>
+  </si>
+  <si>
+    <t>Species found 1979-2019</t>
+  </si>
+  <si>
+    <t>Synonym recorded in 1979, 1999</t>
+  </si>
+  <si>
+    <t>Endemism Status</t>
+  </si>
+  <si>
+    <t>Alisma plantago-aquatica</t>
+  </si>
+  <si>
+    <t>Iris pseudacorus</t>
+  </si>
+  <si>
+    <t>Llilaeopsis occidentalis</t>
+  </si>
+  <si>
+    <t>Lysichiton americanus</t>
+  </si>
+  <si>
+    <t>Platanthera dilatata var dilatata</t>
+  </si>
+  <si>
+    <t>Trifolium wormskioldii</t>
+  </si>
+  <si>
+    <t>Exotic</t>
+  </si>
+  <si>
+    <t>Native</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA </t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Carex </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sp1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Carex </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sp2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Composite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (unidentified)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Festuca </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Galium</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Grass</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(unidentified)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Salix </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sp</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1098,7 +1194,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1202,6 +1298,19 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1407,7 +1516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1785,6 +1894,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1824,15 +1942,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2147,11 +2269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625F1577-DE26-4051-92E5-B0BE0DA6AC79}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2202,7 +2323,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
         <v>83</v>
       </c>
@@ -2218,7 +2339,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>85</v>
       </c>
@@ -2232,7 +2353,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
       <c r="B5" s="30" t="s">
         <v>87</v>
@@ -2246,7 +2367,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="155" t="s">
         <v>89</v>
       </c>
@@ -2265,7 +2386,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
         <v>21</v>
       </c>
@@ -2283,7 +2404,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>92</v>
       </c>
@@ -2301,7 +2422,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="9" t="s">
         <v>94</v>
@@ -2315,7 +2436,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
       <c r="B10" s="21" t="s">
         <v>96</v>
@@ -2329,7 +2450,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="29" t="s">
         <v>3</v>
       </c>
@@ -2365,7 +2486,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="29" t="s">
         <v>27</v>
       </c>
@@ -2381,7 +2502,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>102</v>
       </c>
@@ -2395,7 +2516,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="29" t="s">
         <v>32</v>
       </c>
@@ -2413,7 +2534,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="26" t="s">
@@ -2427,7 +2548,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="29" t="s">
         <v>10</v>
       </c>
@@ -2445,7 +2566,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -2461,7 +2582,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="29" t="s">
         <v>31</v>
       </c>
@@ -2495,7 +2616,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>111</v>
       </c>
@@ -2509,7 +2630,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="21"/>
       <c r="B22" s="33"/>
       <c r="C22" s="26" t="s">
@@ -2523,7 +2644,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="29" t="s">
         <v>115</v>
       </c>
@@ -2541,7 +2662,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="21"/>
       <c r="B24" s="2" t="s">
         <v>117</v>
@@ -2555,7 +2676,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="29" t="s">
         <v>26</v>
       </c>
@@ -2571,7 +2692,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>120</v>
       </c>
@@ -2587,7 +2708,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="29"/>
       <c r="B27" s="29"/>
       <c r="C27" s="37" t="s">
@@ -2635,7 +2756,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="26" t="s">
@@ -2649,7 +2770,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="29" t="s">
         <v>13</v>
       </c>
@@ -2667,7 +2788,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>130</v>
       </c>
@@ -2683,7 +2804,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="29" t="s">
         <v>73</v>
       </c>
@@ -2701,7 +2822,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>24</v>
       </c>
@@ -2719,7 +2840,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="29" t="s">
         <v>75</v>
       </c>
@@ -2735,7 +2856,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>134</v>
       </c>
@@ -2749,7 +2870,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="29" t="s">
         <v>136</v>
       </c>
@@ -2779,7 +2900,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="29"/>
       <c r="B39" s="29" t="s">
         <v>138</v>
@@ -2795,7 +2916,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>9</v>
       </c>
@@ -2869,7 +2990,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>28</v>
       </c>
@@ -2887,7 +3008,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="29" t="s">
         <v>147</v>
       </c>
@@ -2901,7 +3022,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="26"/>
       <c r="C46" s="26" t="s">
@@ -2933,7 +3054,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>152</v>
       </c>
@@ -2967,7 +3088,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>156</v>
       </c>
@@ -2985,7 +3106,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="29" t="s">
         <v>18</v>
       </c>
@@ -3015,7 +3136,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="9"/>
       <c r="B53" s="9" t="s">
         <v>161</v>
@@ -3043,7 +3164,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="29" t="s">
         <v>78</v>
       </c>
@@ -3061,7 +3182,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="155" t="s">
         <v>216</v>
       </c>
@@ -3091,7 +3212,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>170</v>
       </c>
@@ -3109,7 +3230,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="29" t="s">
         <v>16</v>
       </c>
@@ -3127,7 +3248,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
@@ -3141,7 +3262,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="29" t="s">
         <v>22</v>
       </c>
@@ -3159,7 +3280,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>176</v>
       </c>
@@ -3175,7 +3296,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>178</v>
       </c>
@@ -3189,7 +3310,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="B64" s="26"/>
       <c r="C64" s="2" t="s">
@@ -3203,7 +3324,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="29" t="s">
         <v>182</v>
       </c>
@@ -3223,7 +3344,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>25</v>
       </c>
@@ -3241,7 +3362,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="29" t="s">
         <v>185</v>
       </c>
@@ -3271,7 +3392,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="29" t="s">
         <v>189</v>
       </c>
@@ -3289,7 +3410,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
@@ -3307,7 +3428,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="29" t="s">
         <v>193</v>
       </c>
@@ -3325,7 +3446,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>195</v>
       </c>
@@ -3340,13 +3461,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G72" xr:uid="{7C8DDF9E-B538-4E31-B346-1DDB2758620E}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="exotic"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G72" xr:uid="{7C8DDF9E-B538-4E31-B346-1DDB2758620E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3381,34 +3496,34 @@
       <c r="A4" s="123" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="166">
+      <c r="B4" s="173">
         <v>1979</v>
       </c>
-      <c r="C4" s="166"/>
-      <c r="D4" s="166"/>
-      <c r="E4" s="166"/>
-      <c r="G4" s="166">
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="G4" s="173">
         <v>1999</v>
       </c>
-      <c r="H4" s="166"/>
-      <c r="I4" s="166"/>
-      <c r="J4" s="166"/>
-      <c r="L4" s="166">
+      <c r="H4" s="173"/>
+      <c r="I4" s="173"/>
+      <c r="J4" s="173"/>
+      <c r="L4" s="173">
         <v>2019</v>
       </c>
-      <c r="M4" s="166"/>
-      <c r="N4" s="166"/>
-      <c r="O4" s="166"/>
-      <c r="S4" s="162" t="s">
+      <c r="M4" s="173"/>
+      <c r="N4" s="173"/>
+      <c r="O4" s="173"/>
+      <c r="S4" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="T4" s="162"/>
+      <c r="T4" s="169"/>
       <c r="U4" s="113"/>
-      <c r="V4" s="162" t="s">
+      <c r="V4" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="W4" s="162"/>
-      <c r="X4" s="162"/>
+      <c r="W4" s="169"/>
+      <c r="X4" s="169"/>
     </row>
     <row r="5" spans="1:24" ht="39" x14ac:dyDescent="0.35">
       <c r="A5" s="44" t="s">
@@ -4178,24 +4293,24 @@
       <c r="A19" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="166">
+      <c r="B19" s="173">
         <v>1979</v>
       </c>
-      <c r="C19" s="166"/>
-      <c r="D19" s="166"/>
-      <c r="E19" s="166"/>
-      <c r="G19" s="166">
+      <c r="C19" s="173"/>
+      <c r="D19" s="173"/>
+      <c r="E19" s="173"/>
+      <c r="G19" s="173">
         <v>1999</v>
       </c>
-      <c r="H19" s="166"/>
-      <c r="I19" s="166"/>
-      <c r="J19" s="166"/>
-      <c r="L19" s="166">
+      <c r="H19" s="173"/>
+      <c r="I19" s="173"/>
+      <c r="J19" s="173"/>
+      <c r="L19" s="173">
         <v>2019</v>
       </c>
-      <c r="M19" s="166"/>
-      <c r="N19" s="166"/>
-      <c r="O19" s="166"/>
+      <c r="M19" s="173"/>
+      <c r="N19" s="173"/>
+      <c r="O19" s="173"/>
       <c r="R19" s="116">
         <v>2019</v>
       </c>
@@ -4780,24 +4895,24 @@
       <c r="A34" s="123" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="166">
+      <c r="B34" s="173">
         <v>1979</v>
       </c>
-      <c r="C34" s="166"/>
-      <c r="D34" s="166"/>
-      <c r="E34" s="166"/>
-      <c r="G34" s="166">
+      <c r="C34" s="173"/>
+      <c r="D34" s="173"/>
+      <c r="E34" s="173"/>
+      <c r="G34" s="173">
         <v>1999</v>
       </c>
-      <c r="H34" s="166"/>
-      <c r="I34" s="166"/>
-      <c r="J34" s="166"/>
-      <c r="L34" s="166">
+      <c r="H34" s="173"/>
+      <c r="I34" s="173"/>
+      <c r="J34" s="173"/>
+      <c r="L34" s="173">
         <v>2019</v>
       </c>
-      <c r="M34" s="166"/>
-      <c r="N34" s="166"/>
-      <c r="O34" s="166"/>
+      <c r="M34" s="173"/>
+      <c r="N34" s="173"/>
+      <c r="O34" s="173"/>
     </row>
     <row r="35" spans="1:15" ht="39" x14ac:dyDescent="0.35">
       <c r="A35" s="44" t="s">
@@ -5290,24 +5405,24 @@
       <c r="A49" s="123" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="166">
+      <c r="B49" s="173">
         <v>1979</v>
       </c>
-      <c r="C49" s="166"/>
-      <c r="D49" s="166"/>
-      <c r="E49" s="166"/>
-      <c r="G49" s="166">
+      <c r="C49" s="173"/>
+      <c r="D49" s="173"/>
+      <c r="E49" s="173"/>
+      <c r="G49" s="173">
         <v>1999</v>
       </c>
-      <c r="H49" s="166"/>
-      <c r="I49" s="166"/>
-      <c r="J49" s="166"/>
-      <c r="L49" s="166">
+      <c r="H49" s="173"/>
+      <c r="I49" s="173"/>
+      <c r="J49" s="173"/>
+      <c r="L49" s="173">
         <v>2019</v>
       </c>
-      <c r="M49" s="166"/>
-      <c r="N49" s="166"/>
-      <c r="O49" s="166"/>
+      <c r="M49" s="173"/>
+      <c r="N49" s="173"/>
+      <c r="O49" s="173"/>
     </row>
     <row r="50" spans="1:15" ht="39" x14ac:dyDescent="0.35">
       <c r="A50" s="44" t="s">
@@ -5900,7 +6015,7 @@
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C4" s="167" t="s">
+      <c r="C4" s="174" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="129" t="s">
@@ -5917,7 +6032,7 @@
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C5" s="168"/>
+      <c r="C5" s="175"/>
       <c r="D5" s="130" t="s">
         <v>211</v>
       </c>
@@ -5932,7 +6047,7 @@
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C6" s="169" t="s">
+      <c r="C6" s="176" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="142" t="s">
@@ -5949,7 +6064,7 @@
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C7" s="168"/>
+      <c r="C7" s="175"/>
       <c r="D7" s="143" t="s">
         <v>211</v>
       </c>
@@ -5964,7 +6079,7 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C8" s="167" t="s">
+      <c r="C8" s="174" t="s">
         <v>44</v>
       </c>
       <c r="D8" s="142" t="s">
@@ -5981,7 +6096,7 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C9" s="168"/>
+      <c r="C9" s="175"/>
       <c r="D9" s="143" t="s">
         <v>211</v>
       </c>
@@ -6007,808 +6122,1256 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F0E501D-E36F-4F14-87D7-20731F77FBF1}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="179"/>
+    <col min="2" max="2" width="30.26953125" style="180" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" style="180" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="179" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1">
+        <v>1999</v>
+      </c>
+      <c r="F1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1">
+        <v>1979</v>
+      </c>
+      <c r="H1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="178" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="177" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="181" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="183" t="s">
+        <v>305</v>
+      </c>
+      <c r="E2" s="157" t="s">
+        <v>290</v>
+      </c>
+      <c r="F2" s="159" t="s">
+        <v>289</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="H2" s="159" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="179" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="182" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" s="158"/>
+      <c r="D3" s="179" t="s">
+        <v>305</v>
+      </c>
+      <c r="E3" s="157" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" s="157"/>
+      <c r="G3" s="9" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="178" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="181" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="177"/>
+      <c r="D4" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="E4" s="157" t="s">
+        <v>286</v>
+      </c>
+      <c r="F4" s="157" t="s">
+        <v>285</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="179" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="158" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="158"/>
+      <c r="D5" s="179" t="s">
+        <v>306</v>
+      </c>
+      <c r="E5" s="157" t="s">
+        <v>284</v>
+      </c>
+      <c r="F5" s="157"/>
+      <c r="G5" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="H5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="178" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="177" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="177"/>
+      <c r="D6" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E6" s="157" t="s">
+        <v>282</v>
+      </c>
+      <c r="F6" s="157"/>
+      <c r="G6" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="178" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="177" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="181"/>
+      <c r="D7" s="183" t="s">
+        <v>306</v>
+      </c>
+      <c r="E7" s="157" t="s">
+        <v>283</v>
+      </c>
+      <c r="F7" s="157"/>
+      <c r="G7" s="9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="178"/>
+      <c r="B8" s="181" t="s">
+        <v>309</v>
+      </c>
+      <c r="C8" s="177"/>
+      <c r="D8" s="178" t="s">
+        <v>307</v>
+      </c>
+      <c r="E8" s="157" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="157"/>
+      <c r="G8" s="9" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="178"/>
+      <c r="B9" s="177" t="s">
+        <v>310</v>
+      </c>
+      <c r="C9" s="177"/>
+      <c r="D9" s="178" t="s">
+        <v>307</v>
+      </c>
+      <c r="E9" s="157" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="157"/>
+      <c r="G9" s="9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="178" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="177" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="181"/>
+      <c r="D10" s="183" t="s">
+        <v>305</v>
+      </c>
+      <c r="E10" s="157" t="s">
+        <v>280</v>
+      </c>
+      <c r="F10" s="157"/>
+      <c r="G10" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="178"/>
+      <c r="B11" s="181" t="s">
+        <v>311</v>
+      </c>
+      <c r="C11" s="177"/>
+      <c r="D11" s="178" t="s">
+        <v>308</v>
+      </c>
+      <c r="E11" s="157" t="s">
+        <v>279</v>
+      </c>
+      <c r="F11" s="157"/>
+      <c r="G11" s="9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="178" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="177" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="177"/>
+      <c r="D12" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E12" s="157" t="s">
+        <v>276</v>
+      </c>
+      <c r="F12" s="157"/>
+      <c r="G12" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="178" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="177" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="181"/>
+      <c r="D13" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E13" s="157" t="s">
+        <v>275</v>
+      </c>
+      <c r="F13" s="157"/>
+      <c r="G13" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="178" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="181" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="177"/>
+      <c r="D14" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E14" s="157" t="s">
+        <v>274</v>
+      </c>
+      <c r="F14" s="157"/>
+      <c r="G14" s="9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="178" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="177" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="177"/>
+      <c r="D15" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E15" s="157" t="s">
+        <v>273</v>
+      </c>
+      <c r="F15" s="157"/>
+      <c r="G15" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="178" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="177" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="181"/>
+      <c r="D16" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E16" s="157" t="s">
+        <v>272</v>
+      </c>
+      <c r="F16" s="157"/>
+      <c r="G16" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="178" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="181" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="177"/>
+      <c r="D17" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E17" s="157" t="s">
+        <v>271</v>
+      </c>
+      <c r="F17" s="157"/>
+      <c r="G17" s="9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="178" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="177" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="177"/>
+      <c r="D18" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="E18" s="157" t="s">
+        <v>269</v>
+      </c>
+      <c r="F18" s="157"/>
+      <c r="G18" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="H18" s="159" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="178"/>
+      <c r="B19" s="177" t="s">
+        <v>312</v>
+      </c>
+      <c r="C19" s="181"/>
+      <c r="D19" s="183" t="s">
+        <v>307</v>
+      </c>
+      <c r="E19" s="157" t="s">
+        <v>266</v>
+      </c>
+      <c r="F19" s="157"/>
+      <c r="G19" s="9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="178" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="181" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="177"/>
+      <c r="D20" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E20" s="157" t="s">
+        <v>264</v>
+      </c>
+      <c r="F20" s="157"/>
+      <c r="G20" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="178"/>
+      <c r="B21" s="177" t="s">
         <v>313</v>
       </c>
-      <c r="B1">
-        <v>2019</v>
-      </c>
-      <c r="C1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D1">
-        <v>1999</v>
-      </c>
-      <c r="E1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F1">
-        <v>1979</v>
-      </c>
-      <c r="G1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D2" s="170" t="s">
-        <v>310</v>
-      </c>
-      <c r="E2" s="172" t="s">
-        <v>309</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="G2" s="172" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C21" s="177"/>
+      <c r="D21" s="178" t="s">
+        <v>307</v>
+      </c>
+      <c r="E21" s="157" t="s">
+        <v>262</v>
+      </c>
+      <c r="F21" s="157"/>
+      <c r="G21" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="178" t="s">
+        <v>277</v>
+      </c>
+      <c r="B22" s="177" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="181" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E22" s="157" t="s">
+        <v>261</v>
+      </c>
+      <c r="F22" s="157"/>
+      <c r="G22" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="178"/>
+      <c r="B23" s="181" t="s">
+        <v>314</v>
+      </c>
+      <c r="C23" s="177"/>
+      <c r="D23" s="178" t="s">
+        <v>308</v>
+      </c>
+      <c r="E23" s="157" t="s">
+        <v>260</v>
+      </c>
+      <c r="F23" s="157"/>
+      <c r="G23" s="9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="178" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="177" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="177"/>
+      <c r="D24" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E24" s="157" t="s">
+        <v>258</v>
+      </c>
+      <c r="F24" s="157"/>
+      <c r="G24" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="178" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="177" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="181" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E25" s="157" t="s">
+        <v>257</v>
+      </c>
+      <c r="F25" s="157"/>
+      <c r="G25" s="9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="178" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="181" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="177"/>
+      <c r="D26" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="E26" s="157" t="s">
+        <v>256</v>
+      </c>
+      <c r="F26" s="157"/>
+      <c r="G26" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="178" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="177" t="s">
+        <v>300</v>
+      </c>
+      <c r="C27" s="177"/>
+      <c r="D27" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="E27" s="157" t="s">
+        <v>255</v>
+      </c>
+      <c r="F27" s="157"/>
+      <c r="G27" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="178" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="177" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="181"/>
+      <c r="D28" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E28" s="157" t="s">
+        <v>253</v>
+      </c>
+      <c r="F28" s="157"/>
+      <c r="G28" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="178" t="s">
+        <v>293</v>
+      </c>
+      <c r="B29" s="181" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="177"/>
+      <c r="D29" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E29" s="157" t="s">
+        <v>251</v>
+      </c>
+      <c r="F29" s="157"/>
+      <c r="G29" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="178" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="177" t="s">
+        <v>130</v>
+      </c>
+      <c r="C30" s="177"/>
+      <c r="D30" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E30" s="157" t="s">
+        <v>250</v>
+      </c>
+      <c r="F30" s="157"/>
+      <c r="G30" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="178" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" s="177" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="181"/>
+      <c r="D31" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E31" s="157" t="s">
+        <v>249</v>
+      </c>
+      <c r="F31" s="157"/>
+      <c r="G31" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="178" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="181" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="177"/>
+      <c r="D32" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E32" s="157" t="s">
+        <v>248</v>
+      </c>
+      <c r="F32" s="159" t="s">
+        <v>247</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="H32" s="159" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="178" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="177" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="177"/>
+      <c r="D33" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E33" s="157" t="s">
+        <v>246</v>
+      </c>
+      <c r="F33" s="157"/>
+      <c r="G33" s="9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="178" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="177" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" s="181"/>
+      <c r="D34" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E34" s="157" t="s">
+        <v>245</v>
+      </c>
+      <c r="F34" s="157"/>
+      <c r="G34" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="178" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="181" t="s">
+        <v>301</v>
+      </c>
+      <c r="C35" s="177"/>
+      <c r="D35" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E35" s="157" t="s">
+        <v>242</v>
+      </c>
+      <c r="F35" s="157"/>
+      <c r="G35" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="178" t="s">
+        <v>218</v>
+      </c>
+      <c r="B36" s="177" t="s">
+        <v>219</v>
+      </c>
+      <c r="C36" s="177"/>
+      <c r="D36" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="E36" s="157" t="s">
+        <v>241</v>
+      </c>
+      <c r="F36" s="157"/>
+      <c r="G36" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="178" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="177" t="s">
+        <v>302</v>
+      </c>
+      <c r="C37" s="181"/>
+      <c r="D37" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E37" s="157" t="s">
+        <v>239</v>
+      </c>
+      <c r="F37" s="157"/>
+      <c r="G37" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="178" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="181" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="177"/>
+      <c r="D38" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E38" s="157" t="s">
+        <v>240</v>
+      </c>
+      <c r="F38" s="157"/>
+      <c r="G38" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="178" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="177" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="177"/>
+      <c r="D39" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="E39" s="157" t="s">
+        <v>235</v>
+      </c>
+      <c r="F39" s="157"/>
+      <c r="G39" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="178" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" s="177" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="181" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="183" t="s">
+        <v>305</v>
+      </c>
+      <c r="E40" s="157" t="s">
+        <v>233</v>
+      </c>
+      <c r="F40" s="157"/>
+      <c r="G40" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="178" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="181" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" s="177"/>
+      <c r="D41" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="E41" s="157" t="s">
+        <v>232</v>
+      </c>
+      <c r="F41" s="157"/>
+      <c r="G41" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="178" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="177" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="177"/>
+      <c r="D42" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E42" s="157" t="s">
+        <v>231</v>
+      </c>
+      <c r="F42" s="157"/>
+      <c r="G42" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="178" t="s">
+        <v>148</v>
+      </c>
+      <c r="B43" s="177" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" s="181"/>
+      <c r="D43" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E43" s="157" t="s">
+        <v>230</v>
+      </c>
+      <c r="F43" s="157"/>
+      <c r="G43" s="9" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="178" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" s="181" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="177"/>
+      <c r="D44" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="E44" s="157" t="s">
+        <v>228</v>
+      </c>
+      <c r="F44" s="157" t="s">
+        <v>227</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="178" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" s="177" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" s="177"/>
+      <c r="D45" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E45" s="157" t="s">
+        <v>234</v>
+      </c>
+      <c r="F45" s="157"/>
+      <c r="G45" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="178" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" s="177" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="181"/>
+      <c r="D46" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E46" s="157" t="s">
+        <v>225</v>
+      </c>
+      <c r="F46" s="157"/>
+      <c r="G46" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="178" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" s="181" t="s">
+        <v>154</v>
+      </c>
+      <c r="C47" s="177"/>
+      <c r="D47" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="E47" s="157" t="s">
+        <v>223</v>
+      </c>
+      <c r="F47" s="157" t="s">
+        <v>222</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="178" t="s">
+        <v>157</v>
+      </c>
+      <c r="B48" s="177" t="s">
+        <v>303</v>
+      </c>
+      <c r="C48" s="177"/>
+      <c r="D48" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="E48" s="157" t="s">
+        <v>221</v>
+      </c>
+      <c r="F48" s="157"/>
+      <c r="G48" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="178" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="177" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="181"/>
+      <c r="D49" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="178" t="s">
+        <v>160</v>
+      </c>
+      <c r="B50" s="181" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" s="177"/>
+      <c r="D50" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H50" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="178" t="s">
+        <v>164</v>
+      </c>
+      <c r="B51" s="177" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" s="177"/>
+      <c r="D51" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="178" t="s">
+        <v>165</v>
+      </c>
+      <c r="B52" s="177" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="181"/>
+      <c r="D52" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="178" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" s="181" t="s">
+        <v>216</v>
+      </c>
+      <c r="C53" s="177"/>
+      <c r="D53" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="178" t="s">
+        <v>169</v>
+      </c>
+      <c r="B54" s="177" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" s="177"/>
+      <c r="D54" s="178" t="s">
+        <v>305</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="H54" s="157" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="178" t="s">
+        <v>171</v>
+      </c>
+      <c r="B55" s="177" t="s">
+        <v>170</v>
+      </c>
+      <c r="C55" s="181"/>
+      <c r="D55" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="178" t="s">
+        <v>172</v>
+      </c>
+      <c r="B56" s="181" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" s="177"/>
+      <c r="D56" s="178" t="s">
+        <v>306</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="178" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57" s="177" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="177"/>
+      <c r="D57" s="178" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="178" t="s">
+        <v>174</v>
+      </c>
+      <c r="B58" s="177" t="s">
+        <v>173</v>
+      </c>
+      <c r="C58" s="181"/>
+      <c r="D58" s="178" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" s="178" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" s="181" t="s">
+        <v>176</v>
+      </c>
+      <c r="C59" s="177"/>
+      <c r="D59" s="178" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" s="178"/>
+      <c r="B60" s="177" t="s">
+        <v>315</v>
+      </c>
+      <c r="C60" s="177"/>
+      <c r="D60" s="178" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="178" t="s">
+        <v>183</v>
+      </c>
+      <c r="B61" s="177" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="181" t="s">
+        <v>182</v>
+      </c>
+      <c r="D61" s="178" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" s="178" t="s">
+        <v>181</v>
+      </c>
+      <c r="B62" s="181" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" s="177"/>
+      <c r="D62" s="178" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" s="178" t="s">
+        <v>184</v>
+      </c>
+      <c r="B63" s="177" t="s">
+        <v>292</v>
+      </c>
+      <c r="C63" s="177"/>
+      <c r="D63" s="178" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" s="178" t="s">
+        <v>186</v>
+      </c>
+      <c r="B64" s="177" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" s="181"/>
+      <c r="D64" s="178" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="178" t="s">
+        <v>188</v>
+      </c>
+      <c r="B65" s="181" t="s">
+        <v>187</v>
+      </c>
+      <c r="C65" s="177"/>
+      <c r="D65" s="178" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="178" t="s">
+        <v>191</v>
+      </c>
+      <c r="B66" s="177" t="s">
+        <v>190</v>
+      </c>
+      <c r="C66" s="177" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66" s="178" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="178" t="s">
+        <v>192</v>
+      </c>
+      <c r="B67" s="177" t="s">
         <v>304</v>
       </c>
-      <c r="D3" s="170" t="s">
-        <v>308</v>
-      </c>
-      <c r="E3" s="170"/>
-      <c r="F3" s="9" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" t="s">
-        <v>303</v>
-      </c>
-      <c r="D4" s="170" t="s">
+      <c r="C67" s="181" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="178" t="s">
         <v>306</v>
       </c>
-      <c r="E4" s="170" t="s">
-        <v>305</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" t="s">
-        <v>302</v>
-      </c>
-      <c r="D5" s="170" t="s">
-        <v>304</v>
-      </c>
-      <c r="E5" s="170"/>
-      <c r="F5" s="9" t="s">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="178" t="s">
+        <v>194</v>
+      </c>
+      <c r="B68" s="181" t="s">
+        <v>193</v>
+      </c>
+      <c r="C68" s="177"/>
+      <c r="D68" s="178" t="s">
         <v>306</v>
       </c>
-      <c r="G5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" t="s">
-        <v>298</v>
-      </c>
-      <c r="D6" s="170" t="s">
-        <v>302</v>
-      </c>
-      <c r="E6" s="170"/>
-      <c r="F6" s="9" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" t="s">
-        <v>291</v>
-      </c>
-      <c r="D7" s="170" t="s">
-        <v>303</v>
-      </c>
-      <c r="E7" s="170"/>
-      <c r="F7" s="9" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" t="s">
-        <v>301</v>
-      </c>
-      <c r="D8" s="170" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="170"/>
-      <c r="F8" s="9" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" t="s">
-        <v>289</v>
-      </c>
-      <c r="D9" s="170" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="170"/>
-      <c r="F9" s="9" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" t="s">
-        <v>284</v>
-      </c>
-      <c r="C10" t="s">
-        <v>299</v>
-      </c>
-      <c r="D10" s="170" t="s">
-        <v>298</v>
-      </c>
-      <c r="E10" s="170"/>
-      <c r="F10" s="9" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" t="s">
-        <v>297</v>
-      </c>
-      <c r="D11" s="170" t="s">
-        <v>296</v>
-      </c>
-      <c r="E11" s="170"/>
-      <c r="F11" s="9" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>294</v>
-      </c>
-      <c r="B12" t="s">
-        <v>293</v>
-      </c>
-      <c r="D12" s="170" t="s">
-        <v>292</v>
-      </c>
-      <c r="E12" s="170"/>
-      <c r="F12" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" t="s">
-        <v>277</v>
-      </c>
-      <c r="D13" s="170" t="s">
-        <v>291</v>
-      </c>
-      <c r="E13" s="170"/>
-      <c r="F13" s="9" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>123</v>
-      </c>
-      <c r="B14" t="s">
-        <v>290</v>
-      </c>
-      <c r="D14" s="170" t="s">
-        <v>289</v>
-      </c>
-      <c r="E14" s="170"/>
-      <c r="F14" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" t="s">
-        <v>274</v>
-      </c>
-      <c r="D15" s="170" t="s">
-        <v>288</v>
-      </c>
-      <c r="E15" s="170"/>
-      <c r="F15" s="9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" t="s">
-        <v>287</v>
-      </c>
-      <c r="D16" s="170" t="s">
-        <v>286</v>
-      </c>
-      <c r="E16" s="170"/>
-      <c r="F16" s="9" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" t="s">
-        <v>285</v>
-      </c>
-      <c r="D17" s="170" t="s">
-        <v>284</v>
-      </c>
-      <c r="E17" s="170"/>
-      <c r="F17" s="9" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" t="s">
-        <v>270</v>
-      </c>
-      <c r="C18" t="s">
-        <v>282</v>
-      </c>
-      <c r="D18" s="170" t="s">
-        <v>281</v>
-      </c>
-      <c r="E18" s="170"/>
-      <c r="F18" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="G18" s="172" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" t="s">
-        <v>269</v>
-      </c>
-      <c r="D19" s="170" t="s">
-        <v>278</v>
-      </c>
-      <c r="E19" s="170"/>
-      <c r="F19" s="9" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" t="s">
-        <v>268</v>
-      </c>
-      <c r="D20" s="170" t="s">
-        <v>276</v>
-      </c>
-      <c r="E20" s="170"/>
-      <c r="F20" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="G20" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" t="s">
-        <v>267</v>
-      </c>
-      <c r="D21" s="170" t="s">
-        <v>274</v>
-      </c>
-      <c r="E21" s="170"/>
-      <c r="F21" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>139</v>
-      </c>
-      <c r="B22" t="s">
-        <v>273</v>
-      </c>
-      <c r="D22" s="170" t="s">
-        <v>272</v>
-      </c>
-      <c r="E22" s="170"/>
-      <c r="F22" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>218</v>
-      </c>
-      <c r="B23" s="171" t="s">
-        <v>271</v>
-      </c>
-      <c r="D23" s="170" t="s">
-        <v>270</v>
-      </c>
-      <c r="E23" s="170"/>
-      <c r="F23" s="9" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="171" t="s">
-        <v>258</v>
-      </c>
-      <c r="D24" s="170" t="s">
-        <v>268</v>
-      </c>
-      <c r="E24" s="170"/>
-      <c r="F24" s="9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>140</v>
-      </c>
-      <c r="B25" s="171" t="s">
-        <v>259</v>
-      </c>
-      <c r="D25" s="170" t="s">
-        <v>267</v>
-      </c>
-      <c r="E25" s="170"/>
-      <c r="F25" s="9" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>143</v>
-      </c>
-      <c r="B26" s="171" t="s">
-        <v>266</v>
-      </c>
-      <c r="D26" s="170" t="s">
-        <v>265</v>
-      </c>
-      <c r="E26" s="170"/>
-      <c r="F26" s="9" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>145</v>
-      </c>
-      <c r="B27" s="171" t="s">
-        <v>257</v>
-      </c>
-      <c r="D27" s="170" t="s">
-        <v>264</v>
-      </c>
-      <c r="E27" s="170"/>
-      <c r="F27" s="9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>146</v>
-      </c>
-      <c r="B28" s="171" t="s">
-        <v>253</v>
-      </c>
-      <c r="D28" s="170" t="s">
-        <v>262</v>
-      </c>
-      <c r="E28" s="170"/>
-      <c r="F28" s="9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>150</v>
-      </c>
-      <c r="B29" s="171" t="s">
-        <v>260</v>
-      </c>
-      <c r="D29" s="170" t="s">
-        <v>259</v>
-      </c>
-      <c r="E29" s="170"/>
-      <c r="F29" s="9" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>151</v>
-      </c>
-      <c r="B30" s="171" t="s">
-        <v>250</v>
-      </c>
-      <c r="D30" s="170" t="s">
-        <v>258</v>
-      </c>
-      <c r="E30" s="170"/>
-      <c r="F30" s="9" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>155</v>
-      </c>
-      <c r="B31" s="171" t="s">
-        <v>248</v>
-      </c>
-      <c r="D31" s="170" t="s">
-        <v>257</v>
-      </c>
-      <c r="E31" s="170"/>
-      <c r="F31" s="9" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>157</v>
-      </c>
-      <c r="B32" s="171" t="s">
-        <v>256</v>
-      </c>
-      <c r="D32" s="170" t="s">
-        <v>255</v>
-      </c>
-      <c r="E32" s="172" t="s">
-        <v>254</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="G32" s="172" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>165</v>
-      </c>
-      <c r="B33" s="171" t="s">
-        <v>238</v>
-      </c>
-      <c r="D33" s="170" t="s">
-        <v>253</v>
-      </c>
-      <c r="E33" s="170"/>
-      <c r="F33" s="9" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>169</v>
-      </c>
-      <c r="B34" s="171" t="s">
-        <v>168</v>
-      </c>
-      <c r="D34" s="170" t="s">
-        <v>252</v>
-      </c>
-      <c r="E34" s="170"/>
-      <c r="F34" s="9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>171</v>
-      </c>
-      <c r="B35" s="171" t="s">
-        <v>233</v>
-      </c>
-      <c r="D35" s="170" t="s">
-        <v>249</v>
-      </c>
-      <c r="E35" s="170"/>
-      <c r="F35" s="9" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>172</v>
-      </c>
-      <c r="B36" s="171" t="s">
-        <v>232</v>
-      </c>
-      <c r="D36" s="170" t="s">
-        <v>248</v>
-      </c>
-      <c r="E36" s="170"/>
-      <c r="F36" s="9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>175</v>
-      </c>
-      <c r="B37" s="171" t="s">
-        <v>231</v>
-      </c>
-      <c r="D37" s="170" t="s">
-        <v>245</v>
-      </c>
-      <c r="E37" s="170"/>
-      <c r="F37" s="9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>174</v>
-      </c>
-      <c r="B38" s="171" t="s">
-        <v>247</v>
-      </c>
-      <c r="D38" s="170" t="s">
-        <v>246</v>
-      </c>
-      <c r="E38" s="170"/>
-      <c r="F38" s="9" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>181</v>
-      </c>
-      <c r="B39" s="171" t="s">
-        <v>244</v>
-      </c>
-      <c r="D39" s="170" t="s">
-        <v>238</v>
-      </c>
-      <c r="E39" s="170"/>
-      <c r="F39" s="9" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>183</v>
-      </c>
-      <c r="B40" s="171" t="s">
-        <v>242</v>
-      </c>
-      <c r="D40" s="170" t="s">
-        <v>233</v>
-      </c>
-      <c r="E40" s="170"/>
-      <c r="F40" s="9" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>184</v>
-      </c>
-      <c r="B41" s="171" t="s">
-        <v>226</v>
-      </c>
-      <c r="D41" s="170" t="s">
-        <v>232</v>
-      </c>
-      <c r="E41" s="170"/>
-      <c r="F41" s="9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>191</v>
-      </c>
-      <c r="B42" s="171" t="s">
-        <v>239</v>
-      </c>
-      <c r="D42" s="170" t="s">
-        <v>231</v>
-      </c>
-      <c r="E42" s="170"/>
-      <c r="F42" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>192</v>
-      </c>
-      <c r="B43" s="171" t="s">
-        <v>237</v>
-      </c>
-      <c r="D43" s="170" t="s">
-        <v>230</v>
-      </c>
-      <c r="E43" s="170"/>
-      <c r="F43" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="G43" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>194</v>
-      </c>
-      <c r="B44" s="171" t="s">
-        <v>221</v>
-      </c>
-      <c r="D44" s="170" t="s">
-        <v>228</v>
-      </c>
-      <c r="E44" s="170" t="s">
-        <v>227</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D45" s="170" t="s">
-        <v>234</v>
-      </c>
-      <c r="E45" s="170"/>
-      <c r="F45" s="9" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D46" s="170" t="s">
-        <v>225</v>
-      </c>
-      <c r="E46" s="170"/>
-      <c r="F46" s="9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D47" s="170" t="s">
-        <v>223</v>
-      </c>
-      <c r="E47" s="170" t="s">
-        <v>222</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D48" s="170" t="s">
-        <v>221</v>
-      </c>
-      <c r="E48" s="170"/>
-      <c r="F48" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="49" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F49" s="9" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="50" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F50" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="G50" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="51" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F51" s="9" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="52" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F52" s="9" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="53" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F53" s="9" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="54" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F54" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="G54" s="170" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="55" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F55" s="9" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="56" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F56" s="9" t="s">
-        <v>220</v>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="178" t="s">
+        <v>196</v>
+      </c>
+      <c r="B69" s="177" t="s">
+        <v>195</v>
+      </c>
+      <c r="C69" s="177"/>
+      <c r="D69" s="178" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C69">
+    <sortCondition ref="B2:B69"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6838,57 +7401,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="168" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
-      <c r="L1" s="161"/>
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="168"/>
+      <c r="G1" s="168"/>
+      <c r="H1" s="168"/>
+      <c r="I1" s="168"/>
+      <c r="J1" s="168"/>
+      <c r="K1" s="168"/>
+      <c r="L1" s="168"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="161"/>
-      <c r="B2" s="161"/>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="161"/>
-      <c r="G2" s="161"/>
-      <c r="H2" s="161"/>
-      <c r="I2" s="161"/>
-      <c r="J2" s="161"/>
-      <c r="K2" s="161"/>
-      <c r="L2" s="161"/>
+      <c r="A2" s="168"/>
+      <c r="B2" s="168"/>
+      <c r="C2" s="168"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="168"/>
+      <c r="F2" s="168"/>
+      <c r="G2" s="168"/>
+      <c r="H2" s="168"/>
+      <c r="I2" s="168"/>
+      <c r="J2" s="168"/>
+      <c r="K2" s="168"/>
+      <c r="L2" s="168"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="98"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="41"/>
-      <c r="B4" s="160">
+      <c r="B4" s="167">
         <v>1979</v>
       </c>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
       <c r="E4" s="42"/>
-      <c r="F4" s="160">
+      <c r="F4" s="167">
         <v>1999</v>
       </c>
-      <c r="G4" s="160"/>
-      <c r="H4" s="160"/>
+      <c r="G4" s="167"/>
+      <c r="H4" s="167"/>
       <c r="I4" s="42"/>
-      <c r="J4" s="160">
+      <c r="J4" s="167">
         <v>2019</v>
       </c>
-      <c r="K4" s="160"/>
-      <c r="L4" s="160"/>
+      <c r="K4" s="167"/>
+      <c r="L4" s="167"/>
     </row>
     <row r="5" spans="1:13" s="71" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A5" s="99" t="s">
@@ -6925,7 +7488,7 @@
     </row>
     <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="157" t="s">
+      <c r="A7" s="164" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="49" t="s">
@@ -6960,7 +7523,7 @@
       <c r="M7" s="57"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="158"/>
+      <c r="A8" s="165"/>
       <c r="B8" s="54" t="s">
         <v>16</v>
       </c>
@@ -6987,7 +7550,7 @@
       <c r="M8" s="57"/>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="159"/>
+      <c r="A9" s="166"/>
       <c r="B9" s="66" t="s">
         <v>17</v>
       </c>
@@ -7012,7 +7575,7 @@
       <c r="M10" s="57"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="157" t="s">
+      <c r="A11" s="164" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="49" t="s">
@@ -7047,7 +7610,7 @@
       <c r="M11" s="57"/>
     </row>
     <row r="12" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="158"/>
+      <c r="A12" s="165"/>
       <c r="B12" s="92" t="s">
         <v>22</v>
       </c>
@@ -7080,7 +7643,7 @@
       <c r="M12" s="57"/>
     </row>
     <row r="13" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="158"/>
+      <c r="A13" s="165"/>
       <c r="B13" s="108" t="s">
         <v>23</v>
       </c>
@@ -7113,7 +7676,7 @@
       <c r="M13" s="57"/>
     </row>
     <row r="14" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="158"/>
+      <c r="A14" s="165"/>
       <c r="B14" s="92" t="s">
         <v>24</v>
       </c>
@@ -7140,9 +7703,9 @@
       <c r="M14" s="57"/>
     </row>
     <row r="15" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="158"/>
+      <c r="A15" s="165"/>
       <c r="B15" s="108" t="s">
-        <v>314</v>
+        <v>292</v>
       </c>
       <c r="C15" s="78">
         <v>0.33100000000000002</v>
@@ -7161,7 +7724,7 @@
       <c r="M15" s="57"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="158"/>
+      <c r="A16" s="165"/>
       <c r="B16" s="77" t="s">
         <v>26</v>
       </c>
@@ -7182,11 +7745,11 @@
       <c r="M16" s="57"/>
     </row>
     <row r="17" spans="1:13" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="159"/>
+      <c r="A17" s="166"/>
       <c r="B17" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="173">
+      <c r="C17" s="160">
         <v>0.26700000000000002</v>
       </c>
       <c r="D17" s="83">
@@ -7207,7 +7770,7 @@
       <c r="M18" s="57"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="164" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="111" t="s">
@@ -7242,7 +7805,7 @@
       <c r="M19" s="57"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="158"/>
+      <c r="A20" s="165"/>
       <c r="B20" s="77" t="s">
         <v>29</v>
       </c>
@@ -7275,7 +7838,7 @@
       <c r="M20" s="57"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="158"/>
+      <c r="A21" s="165"/>
       <c r="B21" s="59" t="s">
         <v>21</v>
       </c>
@@ -7308,7 +7871,7 @@
       <c r="M21" s="57"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="158"/>
+      <c r="A22" s="165"/>
       <c r="B22" s="77" t="s">
         <v>30</v>
       </c>
@@ -7341,7 +7904,7 @@
       <c r="M22" s="57"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="158"/>
+      <c r="A23" s="165"/>
       <c r="B23" s="59" t="s">
         <v>10</v>
       </c>
@@ -7374,7 +7937,7 @@
       <c r="M23" s="57"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="158"/>
+      <c r="A24" s="165"/>
       <c r="B24" s="54" t="s">
         <v>9</v>
       </c>
@@ -7407,7 +7970,7 @@
       <c r="M24" s="57"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="158"/>
+      <c r="A25" s="165"/>
       <c r="B25" s="57"/>
       <c r="C25" s="60"/>
       <c r="D25" s="81"/>
@@ -7428,7 +7991,7 @@
       <c r="M25" s="57"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="158"/>
+      <c r="A26" s="165"/>
       <c r="B26" s="57"/>
       <c r="C26" s="60"/>
       <c r="D26" s="81"/>
@@ -7449,7 +8012,7 @@
       <c r="M26" s="57"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="158"/>
+      <c r="A27" s="165"/>
       <c r="B27" s="57"/>
       <c r="C27" s="60"/>
       <c r="D27" s="81"/>
@@ -7470,7 +8033,7 @@
       <c r="M27" s="57"/>
     </row>
     <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="159"/>
+      <c r="A28" s="166"/>
       <c r="B28" s="65"/>
       <c r="C28" s="68"/>
       <c r="D28" s="83"/>
@@ -7528,48 +8091,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="168" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
+      <c r="F1" s="168"/>
+      <c r="G1" s="168"/>
+      <c r="H1" s="168"/>
+      <c r="I1" s="168"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="161"/>
-      <c r="B2" s="161"/>
-      <c r="C2" s="161"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="161"/>
-      <c r="F2" s="161"/>
-      <c r="G2" s="161"/>
-      <c r="H2" s="161"/>
-      <c r="I2" s="161"/>
+      <c r="A2" s="168"/>
+      <c r="B2" s="168"/>
+      <c r="C2" s="168"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="168"/>
+      <c r="F2" s="168"/>
+      <c r="G2" s="168"/>
+      <c r="H2" s="168"/>
+      <c r="I2" s="168"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="98"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="41"/>
-      <c r="B4" s="160">
+      <c r="B4" s="167">
         <v>1979</v>
       </c>
-      <c r="C4" s="160"/>
+      <c r="C4" s="167"/>
       <c r="D4" s="42"/>
-      <c r="E4" s="160">
+      <c r="E4" s="167">
         <v>1999</v>
       </c>
-      <c r="F4" s="160"/>
+      <c r="F4" s="167"/>
       <c r="G4" s="42"/>
-      <c r="H4" s="160">
+      <c r="H4" s="167">
         <v>2019</v>
       </c>
-      <c r="I4" s="160"/>
+      <c r="I4" s="167"/>
     </row>
     <row r="5" spans="1:10" s="71" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="A5" s="99" t="s">
@@ -7597,7 +8160,7 @@
     </row>
     <row r="6" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="157" t="s">
+      <c r="A7" s="164" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="49" t="s">
@@ -7623,7 +8186,7 @@
       <c r="J7" s="57"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="158"/>
+      <c r="A8" s="165"/>
       <c r="B8" s="54" t="s">
         <v>16</v>
       </c>
@@ -7643,7 +8206,7 @@
       <c r="J8" s="57"/>
     </row>
     <row r="9" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="159"/>
+      <c r="A9" s="166"/>
       <c r="B9" s="66" t="s">
         <v>17</v>
       </c>
@@ -7663,7 +8226,7 @@
       <c r="J10" s="57"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="157" t="s">
+      <c r="A11" s="164" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="49" t="s">
@@ -7689,7 +8252,7 @@
       <c r="J11" s="57"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="158"/>
+      <c r="A12" s="165"/>
       <c r="B12" s="92" t="s">
         <v>22</v>
       </c>
@@ -7713,7 +8276,7 @@
       <c r="J12" s="57"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="158"/>
+      <c r="A13" s="165"/>
       <c r="B13" s="108" t="s">
         <v>23</v>
       </c>
@@ -7737,7 +8300,7 @@
       <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="158"/>
+      <c r="A14" s="165"/>
       <c r="B14" s="92" t="s">
         <v>24</v>
       </c>
@@ -7757,9 +8320,9 @@
       <c r="J14" s="57"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="158"/>
+      <c r="A15" s="165"/>
       <c r="B15" s="108" t="s">
-        <v>314</v>
+        <v>292</v>
       </c>
       <c r="C15" s="81">
         <v>5.7999999999999996E-3</v>
@@ -7773,7 +8336,7 @@
       <c r="J15" s="57"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="158"/>
+      <c r="A16" s="165"/>
       <c r="B16" s="77" t="s">
         <v>26</v>
       </c>
@@ -7789,7 +8352,7 @@
       <c r="J16" s="57"/>
     </row>
     <row r="17" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="159"/>
+      <c r="A17" s="166"/>
       <c r="B17" s="110" t="s">
         <v>27</v>
       </c>
@@ -7809,7 +8372,7 @@
       <c r="J18" s="57"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="164" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="111" t="s">
@@ -7835,7 +8398,7 @@
       <c r="J19" s="57"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="158"/>
+      <c r="A20" s="165"/>
       <c r="B20" s="77" t="s">
         <v>29</v>
       </c>
@@ -7859,7 +8422,7 @@
       <c r="J20" s="57"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="158"/>
+      <c r="A21" s="165"/>
       <c r="B21" s="59" t="s">
         <v>21</v>
       </c>
@@ -7883,7 +8446,7 @@
       <c r="J21" s="57"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="158"/>
+      <c r="A22" s="165"/>
       <c r="B22" s="77" t="s">
         <v>30</v>
       </c>
@@ -7907,7 +8470,7 @@
       <c r="J22" s="57"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="158"/>
+      <c r="A23" s="165"/>
       <c r="B23" s="59" t="s">
         <v>10</v>
       </c>
@@ -7931,7 +8494,7 @@
       <c r="J23" s="57"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="158"/>
+      <c r="A24" s="165"/>
       <c r="B24" s="54" t="s">
         <v>9</v>
       </c>
@@ -7955,7 +8518,7 @@
       <c r="J24" s="57"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="158"/>
+      <c r="A25" s="165"/>
       <c r="B25" s="57"/>
       <c r="C25" s="81"/>
       <c r="D25" s="57"/>
@@ -7971,7 +8534,7 @@
       <c r="J25" s="57"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="158"/>
+      <c r="A26" s="165"/>
       <c r="B26" s="57"/>
       <c r="C26" s="81"/>
       <c r="D26" s="57"/>
@@ -7987,7 +8550,7 @@
       <c r="J26" s="57"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="158"/>
+      <c r="A27" s="165"/>
       <c r="B27" s="57"/>
       <c r="C27" s="81"/>
       <c r="D27" s="57"/>
@@ -8003,7 +8566,7 @@
       <c r="J27" s="57"/>
     </row>
     <row r="28" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="159"/>
+      <c r="A28" s="166"/>
       <c r="B28" s="65"/>
       <c r="C28" s="83"/>
       <c r="D28" s="65"/>
@@ -8061,23 +8624,23 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="41"/>
-      <c r="C2" s="160">
+      <c r="C2" s="167">
         <v>1979</v>
       </c>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
       <c r="F2" s="42"/>
-      <c r="G2" s="160">
+      <c r="G2" s="167">
         <v>1999</v>
       </c>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
       <c r="J2" s="42"/>
-      <c r="K2" s="160">
+      <c r="K2" s="167">
         <v>2019</v>
       </c>
-      <c r="L2" s="160"/>
-      <c r="M2" s="160"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
     </row>
     <row r="3" spans="2:13" s="42" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="B3" s="44" t="s">
@@ -8115,7 +8678,7 @@
     </row>
     <row r="4" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="157" t="s">
+      <c r="B5" s="164" t="s">
         <v>49</v>
       </c>
       <c r="C5" s="49" t="s">
@@ -8149,7 +8712,7 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="158"/>
+      <c r="B6" s="165"/>
       <c r="C6" s="54" t="s">
         <v>16</v>
       </c>
@@ -8181,7 +8744,7 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="158"/>
+      <c r="B7" s="165"/>
       <c r="C7" s="59" t="s">
         <v>17</v>
       </c>
@@ -8201,7 +8764,7 @@
       <c r="M7" s="62"/>
     </row>
     <row r="8" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="159"/>
+      <c r="B8" s="166"/>
       <c r="C8" s="63"/>
       <c r="D8" s="64"/>
       <c r="E8" s="64"/>
@@ -8226,7 +8789,7 @@
       <c r="M9" s="72"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="164" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="49" t="s">
@@ -8260,7 +8823,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="158"/>
+      <c r="B11" s="165"/>
       <c r="C11" s="54" t="s">
         <v>76</v>
       </c>
@@ -8292,7 +8855,7 @@
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="158"/>
+      <c r="B12" s="165"/>
       <c r="C12" s="77" t="s">
         <v>24</v>
       </c>
@@ -8312,7 +8875,7 @@
       <c r="M12" s="76"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="158"/>
+      <c r="B13" s="165"/>
       <c r="C13" s="77" t="s">
         <v>23</v>
       </c>
@@ -8332,7 +8895,7 @@
       <c r="M13" s="151"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="158"/>
+      <c r="B14" s="165"/>
       <c r="C14" s="77" t="s">
         <v>15</v>
       </c>
@@ -8352,7 +8915,7 @@
       <c r="M14" s="62"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="158"/>
+      <c r="B15" s="165"/>
       <c r="C15" s="77" t="s">
         <v>25</v>
       </c>
@@ -8372,7 +8935,7 @@
       <c r="M15" s="62"/>
     </row>
     <row r="16" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="159"/>
+      <c r="B16" s="166"/>
       <c r="C16" s="82" t="s">
         <v>156</v>
       </c>
@@ -8403,7 +8966,7 @@
       <c r="M17" s="72"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="164" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="49" t="s">
@@ -8437,7 +9000,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="158"/>
+      <c r="B19" s="165"/>
       <c r="C19" s="77" t="s">
         <v>12</v>
       </c>
@@ -8469,7 +9032,7 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="158"/>
+      <c r="B20" s="165"/>
       <c r="C20" s="59" t="s">
         <v>13</v>
       </c>
@@ -8501,7 +9064,7 @@
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="158"/>
+      <c r="B21" s="165"/>
       <c r="C21" s="77" t="s">
         <v>30</v>
       </c>
@@ -8533,7 +9096,7 @@
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="158"/>
+      <c r="B22" s="165"/>
       <c r="C22" s="59" t="s">
         <v>9</v>
       </c>
@@ -8565,7 +9128,7 @@
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="158"/>
+      <c r="B23" s="165"/>
       <c r="C23" s="77" t="s">
         <v>20</v>
       </c>
@@ -8597,7 +9160,7 @@
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="158"/>
+      <c r="B24" s="165"/>
       <c r="C24" s="90" t="s">
         <v>136</v>
       </c>
@@ -8629,7 +9192,7 @@
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="158"/>
+      <c r="B25" s="165"/>
       <c r="C25" s="77" t="s">
         <v>8</v>
       </c>
@@ -8661,7 +9224,7 @@
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="158"/>
+      <c r="B26" s="165"/>
       <c r="C26" s="57"/>
       <c r="D26" s="61"/>
       <c r="E26" s="61"/>
@@ -8681,7 +9244,7 @@
       <c r="M26" s="93"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="158"/>
+      <c r="B27" s="165"/>
       <c r="C27" s="57"/>
       <c r="D27" s="60"/>
       <c r="E27" s="61"/>
@@ -8701,7 +9264,7 @@
       <c r="M27" s="93"/>
     </row>
     <row r="28" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="159"/>
+      <c r="B28" s="166"/>
       <c r="C28" s="65"/>
       <c r="D28" s="68"/>
       <c r="E28" s="67"/>
@@ -8772,23 +9335,23 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="41"/>
-      <c r="C2" s="160">
+      <c r="C2" s="167">
         <v>1979</v>
       </c>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
       <c r="F2" s="42"/>
-      <c r="G2" s="160">
+      <c r="G2" s="167">
         <v>1999</v>
       </c>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
       <c r="J2" s="42"/>
-      <c r="K2" s="160">
+      <c r="K2" s="167">
         <v>2019</v>
       </c>
-      <c r="L2" s="160"/>
-      <c r="M2" s="160"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
     </row>
     <row r="3" spans="2:13" s="42" customFormat="1" ht="39" x14ac:dyDescent="0.3">
       <c r="B3" s="44" t="s">
@@ -8826,7 +9389,7 @@
     </row>
     <row r="4" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="157" t="s">
+      <c r="B5" s="164" t="s">
         <v>49</v>
       </c>
       <c r="C5" s="49" t="s">
@@ -8860,7 +9423,7 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="158"/>
+      <c r="B6" s="165"/>
       <c r="C6" s="54" t="s">
         <v>16</v>
       </c>
@@ -8892,7 +9455,7 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="158"/>
+      <c r="B7" s="165"/>
       <c r="C7" s="59" t="s">
         <v>17</v>
       </c>
@@ -8912,7 +9475,7 @@
       <c r="M7" s="62"/>
     </row>
     <row r="8" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="159"/>
+      <c r="B8" s="166"/>
       <c r="C8" s="63"/>
       <c r="D8" s="64"/>
       <c r="E8" s="64"/>
@@ -8937,7 +9500,7 @@
       <c r="M9" s="72"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="164" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="49" t="s">
@@ -8971,7 +9534,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="158"/>
+      <c r="B11" s="165"/>
       <c r="C11" s="54" t="s">
         <v>76</v>
       </c>
@@ -9003,7 +9566,7 @@
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="158"/>
+      <c r="B12" s="165"/>
       <c r="C12" s="77" t="s">
         <v>24</v>
       </c>
@@ -9023,7 +9586,7 @@
       <c r="M12" s="76"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="158"/>
+      <c r="B13" s="165"/>
       <c r="C13" s="77" t="s">
         <v>23</v>
       </c>
@@ -9043,7 +9606,7 @@
       <c r="M13" s="151"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="158"/>
+      <c r="B14" s="165"/>
       <c r="C14" s="77" t="s">
         <v>15</v>
       </c>
@@ -9063,7 +9626,7 @@
       <c r="M14" s="62"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="158"/>
+      <c r="B15" s="165"/>
       <c r="C15" s="77" t="s">
         <v>25</v>
       </c>
@@ -9083,7 +9646,7 @@
       <c r="M15" s="62"/>
     </row>
     <row r="16" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="159"/>
+      <c r="B16" s="166"/>
       <c r="C16" s="82" t="s">
         <v>156</v>
       </c>
@@ -9114,7 +9677,7 @@
       <c r="M17" s="72"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="164" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="49" t="s">
@@ -9148,7 +9711,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="158"/>
+      <c r="B19" s="165"/>
       <c r="C19" s="77" t="s">
         <v>12</v>
       </c>
@@ -9180,7 +9743,7 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="158"/>
+      <c r="B20" s="165"/>
       <c r="C20" s="59" t="s">
         <v>13</v>
       </c>
@@ -9212,7 +9775,7 @@
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="158"/>
+      <c r="B21" s="165"/>
       <c r="C21" s="77" t="s">
         <v>30</v>
       </c>
@@ -9244,7 +9807,7 @@
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="158"/>
+      <c r="B22" s="165"/>
       <c r="C22" s="59" t="s">
         <v>9</v>
       </c>
@@ -9276,7 +9839,7 @@
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="158"/>
+      <c r="B23" s="165"/>
       <c r="C23" s="77" t="s">
         <v>20</v>
       </c>
@@ -9308,7 +9871,7 @@
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="158"/>
+      <c r="B24" s="165"/>
       <c r="C24" s="90" t="s">
         <v>136</v>
       </c>
@@ -9340,7 +9903,7 @@
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="158"/>
+      <c r="B25" s="165"/>
       <c r="C25" s="77" t="s">
         <v>8</v>
       </c>
@@ -9372,7 +9935,7 @@
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="158"/>
+      <c r="B26" s="165"/>
       <c r="C26" s="57"/>
       <c r="D26" s="61"/>
       <c r="E26" s="61"/>
@@ -9392,7 +9955,7 @@
       <c r="M26" s="93"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="158"/>
+      <c r="B27" s="165"/>
       <c r="C27" s="57"/>
       <c r="D27" s="60"/>
       <c r="E27" s="61"/>
@@ -9412,7 +9975,7 @@
       <c r="M27" s="93"/>
     </row>
     <row r="28" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="159"/>
+      <c r="B28" s="166"/>
       <c r="C28" s="65"/>
       <c r="D28" s="68"/>
       <c r="E28" s="67"/>
@@ -9616,68 +10179,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="172" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="J1" s="164" t="s">
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="J1" s="171" t="s">
         <v>206</v>
       </c>
-      <c r="K1" s="164"/>
-      <c r="L1" s="164"/>
-      <c r="M1" s="164"/>
-      <c r="N1" s="164"/>
-      <c r="O1" s="164"/>
-      <c r="P1" s="164"/>
-      <c r="R1" s="164" t="s">
+      <c r="K1" s="171"/>
+      <c r="L1" s="171"/>
+      <c r="M1" s="171"/>
+      <c r="N1" s="171"/>
+      <c r="O1" s="171"/>
+      <c r="P1" s="171"/>
+      <c r="R1" s="171" t="s">
         <v>207</v>
       </c>
-      <c r="S1" s="164"/>
-      <c r="T1" s="164"/>
-      <c r="U1" s="164"/>
-      <c r="V1" s="164"/>
-      <c r="W1" s="164"/>
-      <c r="X1" s="164"/>
+      <c r="S1" s="171"/>
+      <c r="T1" s="171"/>
+      <c r="U1" s="171"/>
+      <c r="V1" s="171"/>
+      <c r="W1" s="171"/>
+      <c r="X1" s="171"/>
     </row>
     <row r="2" spans="2:24" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="43"/>
-      <c r="C2" s="162" t="s">
+      <c r="C2" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="162"/>
+      <c r="D2" s="169"/>
       <c r="E2" s="113"/>
-      <c r="F2" s="162" t="s">
+      <c r="F2" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="K2" s="163" t="s">
+      <c r="G2" s="169"/>
+      <c r="H2" s="169"/>
+      <c r="K2" s="170" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="163"/>
+      <c r="L2" s="170"/>
       <c r="M2" s="43"/>
-      <c r="N2" s="163" t="s">
+      <c r="N2" s="170" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
+      <c r="O2" s="170"/>
+      <c r="P2" s="170"/>
       <c r="Q2" s="43"/>
       <c r="R2" s="43"/>
-      <c r="S2" s="163" t="s">
+      <c r="S2" s="170" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="163"/>
+      <c r="T2" s="170"/>
       <c r="U2" s="43"/>
-      <c r="V2" s="163" t="s">
+      <c r="V2" s="170" t="s">
         <v>40</v>
       </c>
-      <c r="W2" s="163"/>
-      <c r="X2" s="163"/>
+      <c r="W2" s="170"/>
+      <c r="X2" s="170"/>
     </row>
     <row r="3" spans="2:24" s="11" customFormat="1" ht="39" x14ac:dyDescent="0.35">
       <c r="B3" s="44" t="s">
@@ -9950,8 +10513,8 @@
       <c r="D8" s="43"/>
       <c r="E8" s="57"/>
       <c r="F8" s="119"/>
-      <c r="G8" s="174"/>
-      <c r="H8" s="174"/>
+      <c r="G8" s="161"/>
+      <c r="H8" s="161"/>
       <c r="I8" s="132"/>
       <c r="J8" s="132"/>
       <c r="K8" s="132"/>
@@ -9977,18 +10540,18 @@
       <c r="D9" s="43"/>
       <c r="E9" s="57"/>
       <c r="F9" s="119"/>
-      <c r="G9" s="174"/>
-      <c r="H9" s="174"/>
+      <c r="G9" s="161"/>
+      <c r="H9" s="161"/>
       <c r="I9" s="132"/>
-      <c r="J9" s="175" t="s">
+      <c r="J9" s="162" t="s">
         <v>37</v>
       </c>
       <c r="K9" s="137"/>
       <c r="L9" s="137"/>
-      <c r="M9" s="176"/>
-      <c r="N9" s="174"/>
-      <c r="O9" s="174"/>
-      <c r="P9" s="174"/>
+      <c r="M9" s="163"/>
+      <c r="N9" s="161"/>
+      <c r="O9" s="161"/>
+      <c r="P9" s="161"/>
       <c r="Q9" s="132"/>
       <c r="R9" s="42" t="s">
         <v>37</v>
@@ -10209,17 +10772,17 @@
       <c r="E14" s="57"/>
       <c r="F14" s="119"/>
       <c r="G14" s="119"/>
-      <c r="H14" s="174"/>
+      <c r="H14" s="161"/>
       <c r="I14" s="132"/>
-      <c r="J14" s="175" t="s">
+      <c r="J14" s="162" t="s">
         <v>38</v>
       </c>
       <c r="K14" s="137"/>
       <c r="L14" s="137"/>
-      <c r="M14" s="176"/>
-      <c r="N14" s="174"/>
-      <c r="O14" s="174"/>
-      <c r="P14" s="174"/>
+      <c r="M14" s="163"/>
+      <c r="N14" s="161"/>
+      <c r="O14" s="161"/>
+      <c r="P14" s="161"/>
       <c r="Q14" s="132"/>
       <c r="R14" s="42" t="s">
         <v>38</v>
@@ -10426,7 +10989,7 @@
       <c r="J18" s="137"/>
       <c r="K18" s="137"/>
       <c r="L18" s="137"/>
-      <c r="M18" s="176"/>
+      <c r="M18" s="163"/>
       <c r="N18" s="137"/>
       <c r="O18" s="137"/>
       <c r="P18" s="137"/>
@@ -10450,12 +11013,12 @@
       <c r="G19" s="43"/>
       <c r="H19" s="137"/>
       <c r="I19" s="132"/>
-      <c r="J19" s="175" t="s">
+      <c r="J19" s="162" t="s">
         <v>47</v>
       </c>
       <c r="K19" s="137"/>
       <c r="L19" s="137"/>
-      <c r="M19" s="176"/>
+      <c r="M19" s="163"/>
       <c r="N19" s="137"/>
       <c r="O19" s="137"/>
       <c r="P19" s="137"/>
@@ -10500,7 +11063,7 @@
       <c r="L20" s="74">
         <v>47.6</v>
       </c>
-      <c r="M20" s="176"/>
+      <c r="M20" s="163"/>
       <c r="N20" s="120">
         <v>12.153</v>
       </c>
@@ -10561,7 +11124,7 @@
       <c r="L21" s="134">
         <v>42.1</v>
       </c>
-      <c r="M21" s="176"/>
+      <c r="M21" s="163"/>
       <c r="N21" s="121">
         <v>10.023</v>
       </c>
@@ -10622,7 +11185,7 @@
       <c r="L22" s="74">
         <v>41.7</v>
       </c>
-      <c r="M22" s="176"/>
+      <c r="M22" s="163"/>
       <c r="N22" s="120">
         <v>8.1770000000000014</v>
       </c>
@@ -10703,34 +11266,34 @@
       <c r="A4" s="123" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="166">
+      <c r="B4" s="173">
         <v>1979</v>
       </c>
-      <c r="C4" s="166"/>
-      <c r="D4" s="166"/>
-      <c r="E4" s="166"/>
-      <c r="G4" s="166">
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="173"/>
+      <c r="G4" s="173">
         <v>1999</v>
       </c>
-      <c r="H4" s="166"/>
-      <c r="I4" s="166"/>
-      <c r="J4" s="166"/>
-      <c r="L4" s="166">
+      <c r="H4" s="173"/>
+      <c r="I4" s="173"/>
+      <c r="J4" s="173"/>
+      <c r="L4" s="173">
         <v>2019</v>
       </c>
-      <c r="M4" s="166"/>
-      <c r="N4" s="166"/>
-      <c r="O4" s="166"/>
-      <c r="S4" s="162" t="s">
+      <c r="M4" s="173"/>
+      <c r="N4" s="173"/>
+      <c r="O4" s="173"/>
+      <c r="S4" s="169" t="s">
         <v>39</v>
       </c>
-      <c r="T4" s="162"/>
+      <c r="T4" s="169"/>
       <c r="U4" s="113"/>
-      <c r="V4" s="162" t="s">
+      <c r="V4" s="169" t="s">
         <v>40</v>
       </c>
-      <c r="W4" s="162"/>
-      <c r="X4" s="162"/>
+      <c r="W4" s="169"/>
+      <c r="X4" s="169"/>
     </row>
     <row r="5" spans="1:24" ht="39" x14ac:dyDescent="0.35">
       <c r="A5" s="44" t="s">
@@ -11500,24 +12063,24 @@
       <c r="A19" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="166">
+      <c r="B19" s="173">
         <v>1979</v>
       </c>
-      <c r="C19" s="166"/>
-      <c r="D19" s="166"/>
-      <c r="E19" s="166"/>
-      <c r="G19" s="166">
+      <c r="C19" s="173"/>
+      <c r="D19" s="173"/>
+      <c r="E19" s="173"/>
+      <c r="G19" s="173">
         <v>1999</v>
       </c>
-      <c r="H19" s="166"/>
-      <c r="I19" s="166"/>
-      <c r="J19" s="166"/>
-      <c r="L19" s="166">
+      <c r="H19" s="173"/>
+      <c r="I19" s="173"/>
+      <c r="J19" s="173"/>
+      <c r="L19" s="173">
         <v>2019</v>
       </c>
-      <c r="M19" s="166"/>
-      <c r="N19" s="166"/>
-      <c r="O19" s="166"/>
+      <c r="M19" s="173"/>
+      <c r="N19" s="173"/>
+      <c r="O19" s="173"/>
       <c r="R19" s="116">
         <v>2019</v>
       </c>
@@ -12102,24 +12665,24 @@
       <c r="A34" s="123" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="166">
+      <c r="B34" s="173">
         <v>1979</v>
       </c>
-      <c r="C34" s="166"/>
-      <c r="D34" s="166"/>
-      <c r="E34" s="166"/>
-      <c r="G34" s="166">
+      <c r="C34" s="173"/>
+      <c r="D34" s="173"/>
+      <c r="E34" s="173"/>
+      <c r="G34" s="173">
         <v>1999</v>
       </c>
-      <c r="H34" s="166"/>
-      <c r="I34" s="166"/>
-      <c r="J34" s="166"/>
-      <c r="L34" s="166">
+      <c r="H34" s="173"/>
+      <c r="I34" s="173"/>
+      <c r="J34" s="173"/>
+      <c r="L34" s="173">
         <v>2019</v>
       </c>
-      <c r="M34" s="166"/>
-      <c r="N34" s="166"/>
-      <c r="O34" s="166"/>
+      <c r="M34" s="173"/>
+      <c r="N34" s="173"/>
+      <c r="O34" s="173"/>
     </row>
     <row r="35" spans="1:15" ht="39" x14ac:dyDescent="0.35">
       <c r="A35" s="44" t="s">
@@ -12612,24 +13175,24 @@
       <c r="A49" s="123" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="166">
+      <c r="B49" s="173">
         <v>1979</v>
       </c>
-      <c r="C49" s="166"/>
-      <c r="D49" s="166"/>
-      <c r="E49" s="166"/>
-      <c r="G49" s="166">
+      <c r="C49" s="173"/>
+      <c r="D49" s="173"/>
+      <c r="E49" s="173"/>
+      <c r="G49" s="173">
         <v>1999</v>
       </c>
-      <c r="H49" s="166"/>
-      <c r="I49" s="166"/>
-      <c r="J49" s="166"/>
-      <c r="L49" s="166">
+      <c r="H49" s="173"/>
+      <c r="I49" s="173"/>
+      <c r="J49" s="173"/>
+      <c r="L49" s="173">
         <v>2019</v>
       </c>
-      <c r="M49" s="166"/>
-      <c r="N49" s="166"/>
-      <c r="O49" s="166"/>
+      <c r="M49" s="173"/>
+      <c r="N49" s="173"/>
+      <c r="O49" s="173"/>
     </row>
     <row r="50" spans="1:15" ht="39" x14ac:dyDescent="0.35">
       <c r="A50" s="44" t="s">
@@ -13354,18 +13917,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13388,26 +13951,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{672CF68E-CAEE-413A-A4ED-E0B11FCCA037}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D870C599-734A-4F80-B43A-AAD654208358}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{672CF68E-CAEE-413A-A4ED-E0B11FCCA037}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>